<commit_message>
Updating batch file for script installation. Updating gitignore to ignore xlsx files
</commit_message>
<xml_diff>
--- a/unittests/Testing_PrintSettings.xlsx
+++ b/unittests/Testing_PrintSettings.xlsx
@@ -1,36 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Quality Data\Data Technician\eCase Migration\Testing\unittests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sheet'!1:1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet!1:1</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>filler</t>
+  </si>
+  <si>
+    <t>There should be two SAV logos, one above this text and one below.</t>
+  </si>
+  <si>
+    <t>The document should be landscape, and the printview shouldgo to column J</t>
+  </si>
+  <si>
+    <t>The columns are set as [1, 2, 4, 8, 16, 32, 16, 21, 30, .5]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,68 +70,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2381250" cy="381000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2381250" cy="381000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="Picture"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2381250" cy="381000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2381250" cy="381000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr="Picture"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,63 +431,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="C2:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="1" customWidth="1" min="1" max="1"/>
-    <col width="2" customWidth="1" min="2" max="2"/>
-    <col width="4" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="32" customWidth="1" min="6" max="6"/>
-    <col width="16" customWidth="1" min="7" max="7"/>
-    <col width="21" customWidth="1" min="8" max="8"/>
-    <col width="30" customWidth="1" min="9" max="9"/>
-    <col width="0.5" customWidth="1" min="10" max="10"/>
+    <col min="1" max="1" width="1" customWidth="1"/>
+    <col min="2" max="2" width="2" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="10" max="10" width="0.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>filler</t>
-        </is>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>There should be two SAV logos, one above this text and one below.</t>
-        </is>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>The columns are set as [1, 2, 4, 8, 16, 32, 64, 128, 256, 512]</t>
-        </is>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>The document should be landscape, and the printview shouldgo to column J</t>
-        </is>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Error Handling for ecase_downloader.py, if the reports have disappeared from ecase report generator. Added updated requirements.txt file aswell.
</commit_message>
<xml_diff>
--- a/unittests/Testing_PrintSettings.xlsx
+++ b/unittests/Testing_PrintSettings.xlsx
@@ -1,57 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Quality Data\Data Technician\eCase Migration\Testing\unittests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="7740"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet!1:1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sheet'!1:1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>filler</t>
-  </si>
-  <si>
-    <t>There should be two SAV logos, one above this text and one below.</t>
-  </si>
-  <si>
-    <t>The document should be landscape, and the printview shouldgo to column J</t>
-  </si>
-  <si>
-    <t>The columns are set as [1, 2, 4, 8, 16, 32, 16, 21, 30, .5]</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,81 +49,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2381250" cy="381000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="Picture"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2381250" cy="381000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2381250" cy="381000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2" descr="Picture"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2381250" cy="381000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,54 +397,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="C2:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1" customWidth="1"/>
-    <col min="2" max="2" width="2" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="0.42578125" customWidth="1"/>
+    <col width="1" customWidth="1" min="1" max="1"/>
+    <col width="2" customWidth="1" min="2" max="2"/>
+    <col width="4" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="32" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="0.5" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J2" t="s">
-        <v>0</v>
+    <row r="2">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>filler</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>1</v>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>There should be two SAV logos, one above this text and one below.</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>3</v>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The columns are set as [1, 2, 4, 8, 16, 32, 64, 128, 256, 512]</t>
+        </is>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>2</v>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>The document should be landscape, and the printview shouldgo to column J</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>